<commit_message>
Table 1 reproduction of base (steps=0) code and results
</commit_message>
<xml_diff>
--- a/repro_results/T1-GTR.xlsx
+++ b/repro_results/T1-GTR.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Steps</t>
   </si>
@@ -41,12 +41,6 @@
   </si>
   <si>
     <t>Peak Memory (MB)</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>-%</t>
   </si>
 </sst>
 </file>
@@ -54,8 +48,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##0.000"/>
-    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -252,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -274,10 +268,13 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="19" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -286,20 +283,14 @@
     <xf borderId="8" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="1" numFmtId="19" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="19" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -307,13 +298,13 @@
     <xf borderId="11" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="19" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -658,57 +649,57 @@
       <c r="C3" s="6">
         <v>32.0</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>10</v>
+      <c r="D3" s="6">
+        <v>31.0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.315608888237815</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.670728230590925</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.014</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.899243414402008</v>
+      </c>
+      <c r="I3" s="8">
+        <v>6.828703703703704E-4</v>
+      </c>
+      <c r="J3" s="9">
+        <v>9.923254</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9">
+      <c r="A4" s="10">
         <v>1.0</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="11">
         <v>1.0</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="11">
         <v>32.0</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="11">
         <v>31.0</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="12">
         <v>0.495145152166149</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="12">
         <v>0.796588606301905</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="12">
         <v>0.084</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="12">
         <v>0.953415513038635</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="13">
         <v>9.837962962962962E-4</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="14">
         <v>9.930763</v>
       </c>
     </row>
@@ -725,54 +716,54 @@
       <c r="D5" s="6">
         <v>31.0</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="7">
         <v>0.832927019</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="7">
         <v>0.953416225</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="7">
         <v>0.578</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="7">
         <v>0.989138544</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="8">
         <v>0.005891203703703704</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="9">
         <v>9.939087</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="9">
+      <c r="A6" s="10">
         <v>50.0</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="11">
         <v>1.0</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="11">
         <v>32.0</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="11">
         <v>31.0</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="12">
         <v>0.841622796</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="12">
         <v>0.956910759</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="12">
         <v>0.586</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="12">
         <v>0.989138544</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="13">
         <v>0.013506944444444445</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="14">
         <v>9.96747</v>
       </c>
     </row>
@@ -789,86 +780,86 @@
       <c r="D7" s="6">
         <v>31.0</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="7">
         <v>0.871295465060873</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="7">
         <v>0.964604850884493</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="7">
         <v>0.672</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="7">
         <v>0.991714477539062</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="8">
         <v>0.023854166666666666</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="9">
         <v>10.713679</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9">
+      <c r="A8" s="10">
         <v>50.0</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="11">
         <v>4.0</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="11">
         <v>32.0</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="11">
         <v>31.0</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="12">
         <v>0.900075840324615</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="12">
         <v>0.970646892167135</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="12">
         <v>0.75</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="12">
         <v>0.995254158973693</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="13">
         <v>0.04920138888888889</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="14">
         <v>9.884516</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <v>50.0</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>8.0</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="16">
         <v>32.0</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>31.0</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <v>0.923384953</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <v>0.977206298</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="17">
         <v>0.794</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="17">
         <v>0.995254159</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="18">
         <v>0.15444444444444444</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="19">
         <v>10.312106</v>
       </c>
     </row>

</xml_diff>